<commit_message>
Removing the commented code from test class , after confirming the optimizaed code fetch from sheets
</commit_message>
<xml_diff>
--- a/yt_multi_language_ui_validator/src/main/resources/data/ApplicableLanguageExpectedAttibute.xlsx
+++ b/yt_multi_language_ui_validator/src/main/resources/data/ApplicableLanguageExpectedAttibute.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sagar\youtube-multi-language-ui-validator-automation\yt_multi_language_ui_validator\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483E239F-6416-47B1-8EB7-4A3E622E9934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945F0CF1-DEDC-44D6-8723-BA2C21715A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attribute" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -669,7 +669,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>